<commit_message>
nyicil untag. kapan lah selesainya ini...
</commit_message>
<xml_diff>
--- a/pesantren/modul-komputer-mabaiz/penilaian.xlsx
+++ b/pesantren/modul-komputer-mabaiz/penilaian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN PROJECT\zen\pesantren\modul-komputer-mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CA308E-A92E-4945-97ED-4D842EAF96C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405F7A9E-4741-4BD5-BEC8-5CC527F93028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{9BA5602F-5C25-419E-8CF4-DFBBBCF94239}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Nama</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>MENGETIK 10 JARI</t>
+  </si>
+  <si>
+    <t>Aisyah</t>
+  </si>
+  <si>
+    <t>3 Agustus 2023</t>
+  </si>
+  <si>
+    <t>Amila</t>
+  </si>
+  <si>
+    <t>Putri</t>
   </si>
 </sst>
 </file>
@@ -99,10 +111,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,7 +433,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,40 +443,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -487,9 +499,15 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>81</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -501,9 +519,15 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45.2</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -515,9 +539,15 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10.4</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>

</xml_diff>

<commit_message>
tambah hazwan dan kholid
</commit_message>
<xml_diff>
--- a/pesantren/modul-komputer-mabaiz/penilaian.xlsx
+++ b/pesantren/modul-komputer-mabaiz/penilaian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN PROJECT\zen\pesantren\modul-komputer-mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C47BB00-9A6C-4470-8E30-E0B3683E02CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6804CAED-5480-4143-8C0E-891983C067A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{9BA5602F-5C25-419E-8CF4-DFBBBCF94239}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Nama</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>8 Agustus 2023</t>
+  </si>
+  <si>
+    <t>Hazwan</t>
+  </si>
+  <si>
+    <t>Kholid</t>
+  </si>
+  <si>
+    <t>9 Agustus 2023</t>
   </si>
 </sst>
 </file>
@@ -454,7 +463,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,13 +550,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
-        <v>76</v>
+        <v>38.9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -561,13 +570,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -581,13 +590,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2">
-        <v>10.4</v>
+        <v>89.2</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -601,13 +610,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
-        <v>94.7</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -621,13 +630,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
-        <v>90</v>
+        <v>10.4</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -641,13 +650,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>71</v>
+        <v>94.7</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -661,13 +670,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -680,9 +689,15 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>71</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -694,9 +709,15 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>80</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -792,8 +813,8 @@
       <c r="L19" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C11">
-    <sortCondition ref="A3:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
sudah komputer hari ini
</commit_message>
<xml_diff>
--- a/pesantren/modul-komputer-mabaiz/penilaian.xlsx
+++ b/pesantren/modul-komputer-mabaiz/penilaian.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN PROJECT\zen\pesantren\modul-komputer-mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F136A82-289B-4CA0-AE9C-4F51FC531C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1696E45C-3952-4888-A3D6-AF759DA7BEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="-11640" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="الاثنين" sheetId="5" r:id="rId1"/>
-    <sheet name="الأربعاء" sheetId="1" r:id="rId2"/>
-    <sheet name="الخميس" sheetId="2" r:id="rId3"/>
-    <sheet name="الجمعة" sheetId="4" r:id="rId4"/>
+    <sheet name="الثلاثاء" sheetId="6" r:id="rId2"/>
+    <sheet name="الأربعاء" sheetId="1" r:id="rId3"/>
+    <sheet name="الخميس" sheetId="2" r:id="rId4"/>
+    <sheet name="الجمعة" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>اسم</t>
   </si>
@@ -144,9 +145,6 @@
     <t>Zufar</t>
   </si>
   <si>
-    <t>Amar</t>
-  </si>
-  <si>
     <t>Kamil</t>
   </si>
   <si>
@@ -162,7 +160,31 @@
     <t>Fahri</t>
   </si>
   <si>
-    <t>Selasa</t>
+    <t>Akmal</t>
+  </si>
+  <si>
+    <t>Ammar</t>
+  </si>
+  <si>
+    <t>Idris</t>
+  </si>
+  <si>
+    <t>Ifroyim</t>
+  </si>
+  <si>
+    <t>Kholis</t>
+  </si>
+  <si>
+    <t>Fahrezy</t>
+  </si>
+  <si>
+    <t>Faisal</t>
+  </si>
+  <si>
+    <t>Syahid</t>
+  </si>
+  <si>
+    <t>Rizki</t>
   </si>
 </sst>
 </file>
@@ -220,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -260,6 +282,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A19D3B-2FDF-4B23-B1AA-93203B194380}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
@@ -554,69 +582,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -692,11 +720,11 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="12"/>
+      <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7">
         <v>100</v>
@@ -731,7 +759,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="9">
         <v>90</v>
@@ -801,7 +829,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2">
         <v>100</v>
@@ -961,7 +989,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7">
         <v>90</v>
@@ -1220,12 +1248,800 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8331428A-620A-44D2-9959-9DECEF50B2C0}">
+  <dimension ref="A1:Y21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:J3" si="0">D3+1</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:S3" si="1">M3+1</f>
+        <v>4</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="R3" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="S3" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>2</v>
+      </c>
+      <c r="V3" s="2">
+        <v>3</v>
+      </c>
+      <c r="W3" s="15"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2">
+        <v>96</v>
+      </c>
+      <c r="D4" s="2">
+        <v>96</v>
+      </c>
+      <c r="E4" s="5">
+        <v>100</v>
+      </c>
+      <c r="F4" s="2">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>96</v>
+      </c>
+      <c r="H4" s="2">
+        <v>96</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="13"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2">
+        <v>90</v>
+      </c>
+      <c r="D5" s="5">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>93</v>
+      </c>
+      <c r="F5" s="3">
+        <v>96</v>
+      </c>
+      <c r="G5" s="3">
+        <v>90</v>
+      </c>
+      <c r="H5" s="2">
+        <v>86</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="13"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="5">
+        <v>90</v>
+      </c>
+      <c r="C6" s="3">
+        <v>86</v>
+      </c>
+      <c r="D6" s="3">
+        <v>86</v>
+      </c>
+      <c r="E6" s="2">
+        <v>90</v>
+      </c>
+      <c r="F6" s="2">
+        <v>96</v>
+      </c>
+      <c r="G6" s="2">
+        <v>96</v>
+      </c>
+      <c r="H6" s="2">
+        <v>86</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="13"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2">
+        <v>96</v>
+      </c>
+      <c r="C7" s="2">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2">
+        <v>86</v>
+      </c>
+      <c r="E7" s="2">
+        <v>90</v>
+      </c>
+      <c r="F7" s="2">
+        <v>86</v>
+      </c>
+      <c r="G7" s="5">
+        <v>83</v>
+      </c>
+      <c r="H7" s="2">
+        <v>86</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="13"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2">
+        <v>86</v>
+      </c>
+      <c r="C8" s="2">
+        <v>86</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>96</v>
+      </c>
+      <c r="F8" s="2">
+        <v>86</v>
+      </c>
+      <c r="G8" s="2">
+        <v>93</v>
+      </c>
+      <c r="H8" s="3">
+        <v>96</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2">
+        <v>86</v>
+      </c>
+      <c r="C9" s="5">
+        <v>83</v>
+      </c>
+      <c r="D9" s="2">
+        <v>86</v>
+      </c>
+      <c r="E9" s="2">
+        <v>86</v>
+      </c>
+      <c r="F9" s="2">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2">
+        <v>80</v>
+      </c>
+      <c r="H9" s="5">
+        <v>80</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2">
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <v>100</v>
+      </c>
+      <c r="D10" s="2">
+        <v>93</v>
+      </c>
+      <c r="E10" s="2">
+        <v>90</v>
+      </c>
+      <c r="F10" s="5">
+        <v>86</v>
+      </c>
+      <c r="G10" s="2">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2">
+        <v>93</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2">
+        <v>93</v>
+      </c>
+      <c r="C11" s="2">
+        <v>96</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2">
+        <v>100</v>
+      </c>
+      <c r="F11" s="2">
+        <v>93</v>
+      </c>
+      <c r="G11" s="2">
+        <v>93</v>
+      </c>
+      <c r="H11" s="2">
+        <v>100</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="3">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2">
+        <v>93</v>
+      </c>
+      <c r="D12" s="2">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2">
+        <v>93</v>
+      </c>
+      <c r="F12" s="2">
+        <v>90</v>
+      </c>
+      <c r="G12" s="2">
+        <v>93</v>
+      </c>
+      <c r="H12" s="2">
+        <v>93</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A12">
+    <sortCondition ref="A4:A12"/>
+  </sortState>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:W3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+      <selection pane="topRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,69 +2050,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1372,11 +2188,11 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="12"/>
+      <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1849,12 +2665,8 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1954,7 +2766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EEBF04-06B9-43E2-90DC-1C2C9DD1F182}">
   <dimension ref="A1:W11"/>
   <sheetViews>
@@ -1969,69 +2781,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -2107,7 +2919,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="12"/>
+      <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2390,7 +3202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FADA61-5C96-4888-B06A-035DB9B01847}">
   <dimension ref="A1:W9"/>
   <sheetViews>
@@ -2405,69 +3217,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12" t="s">
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -2543,7 +3355,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="12"/>
+      <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">

</xml_diff>

<commit_message>
selesai belajar komputer hari ini
</commit_message>
<xml_diff>
--- a/pesantren/modul-komputer-mabaiz/penilaian.xlsx
+++ b/pesantren/modul-komputer-mabaiz/penilaian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN PROJECT\zen\pesantren\modul-komputer-mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1696E45C-3952-4888-A3D6-AF759DA7BEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E88F3-11F5-4126-AE5E-2272DF9B1FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="-11640" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="الاثنين" sheetId="5" r:id="rId1"/>
@@ -1251,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8331428A-620A-44D2-9959-9DECEF50B2C0}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -2768,11 +2768,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74EEBF04-06B9-43E2-90DC-1C2C9DD1F182}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,13 +2946,45 @@
       <c r="H4" s="2">
         <v>86</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="I4" s="2">
+        <v>90</v>
+      </c>
+      <c r="J4" s="2">
+        <v>93</v>
+      </c>
+      <c r="K4" s="2">
+        <v>83</v>
+      </c>
+      <c r="L4" s="5">
+        <v>90</v>
+      </c>
+      <c r="M4" s="2">
+        <v>96</v>
+      </c>
+      <c r="N4" s="2">
+        <v>90</v>
+      </c>
+      <c r="O4" s="2">
+        <v>90</v>
+      </c>
+      <c r="P4" s="7">
+        <v>96</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>86</v>
+      </c>
+      <c r="R4" s="7">
+        <v>90</v>
+      </c>
+      <c r="S4" s="7">
+        <v>90</v>
+      </c>
+      <c r="T4" s="7">
+        <v>87</v>
+      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2979,13 +3011,45 @@
       <c r="H5" s="3">
         <v>100</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="I5" s="3">
+        <v>100</v>
+      </c>
+      <c r="J5" s="2">
+        <v>96</v>
+      </c>
+      <c r="K5" s="3">
+        <v>96</v>
+      </c>
+      <c r="L5" s="3">
+        <v>90</v>
+      </c>
+      <c r="M5" s="2">
+        <v>93</v>
+      </c>
+      <c r="N5" s="3">
+        <v>96</v>
+      </c>
+      <c r="O5" s="3">
+        <v>96</v>
+      </c>
+      <c r="P5" s="7">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>93</v>
+      </c>
+      <c r="R5" s="7">
+        <v>93</v>
+      </c>
+      <c r="S5" s="7">
+        <v>83</v>
+      </c>
+      <c r="T5" s="8">
+        <v>83</v>
+      </c>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -3012,13 +3076,45 @@
       <c r="H6" s="2">
         <v>93</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="I6" s="2">
+        <v>83</v>
+      </c>
+      <c r="J6" s="2">
+        <v>93</v>
+      </c>
+      <c r="K6" s="2">
+        <v>90</v>
+      </c>
+      <c r="L6" s="2">
+        <v>86</v>
+      </c>
+      <c r="M6" s="2">
+        <v>93</v>
+      </c>
+      <c r="N6" s="2">
+        <v>93</v>
+      </c>
+      <c r="O6" s="2">
+        <v>96</v>
+      </c>
+      <c r="P6" s="7">
+        <v>96</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>93</v>
+      </c>
+      <c r="R6" s="7">
+        <v>93</v>
+      </c>
+      <c r="S6" s="8">
+        <v>93</v>
+      </c>
+      <c r="T6" s="7">
+        <v>83</v>
+      </c>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -3045,13 +3141,45 @@
       <c r="H7" s="2">
         <v>100</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="I7" s="2">
+        <v>100</v>
+      </c>
+      <c r="J7" s="2">
+        <v>100</v>
+      </c>
+      <c r="K7" s="5">
+        <v>96</v>
+      </c>
+      <c r="L7" s="2">
+        <v>100</v>
+      </c>
+      <c r="M7" s="5">
+        <v>86</v>
+      </c>
+      <c r="N7" s="2">
+        <v>96</v>
+      </c>
+      <c r="O7" s="5">
+        <v>93</v>
+      </c>
+      <c r="P7" s="7">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>93</v>
+      </c>
+      <c r="R7" s="7">
+        <v>96</v>
+      </c>
+      <c r="S7" s="7">
+        <v>100</v>
+      </c>
+      <c r="T7" s="7">
+        <v>100</v>
+      </c>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3078,13 +3206,43 @@
       <c r="H8" s="2">
         <v>93</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="I8" s="2">
+        <v>90</v>
+      </c>
+      <c r="J8" s="3">
+        <v>93</v>
+      </c>
+      <c r="K8" s="2">
+        <v>86</v>
+      </c>
+      <c r="L8" s="2">
+        <v>83</v>
+      </c>
+      <c r="M8" s="2">
+        <v>83</v>
+      </c>
+      <c r="N8" s="5">
+        <v>80</v>
+      </c>
+      <c r="O8" s="2">
+        <v>86</v>
+      </c>
+      <c r="P8" s="7">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>86</v>
+      </c>
+      <c r="R8" s="9">
+        <v>83</v>
+      </c>
+      <c r="S8" s="9">
+        <v>86</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -3118,6 +3276,14 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3144,13 +3310,43 @@
       <c r="H10" s="2">
         <v>86</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="I10" s="5">
+        <v>80</v>
+      </c>
+      <c r="J10" s="5">
+        <v>83</v>
+      </c>
+      <c r="K10" s="2">
+        <v>80</v>
+      </c>
+      <c r="L10" s="2">
+        <v>80</v>
+      </c>
+      <c r="M10" s="3">
+        <v>83</v>
+      </c>
+      <c r="N10" s="2">
+        <v>83</v>
+      </c>
+      <c r="O10" s="2">
+        <v>83</v>
+      </c>
+      <c r="P10" s="8">
+        <v>83</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>83</v>
+      </c>
+      <c r="R10" s="8">
+        <v>86</v>
+      </c>
+      <c r="S10" s="7">
+        <v>93</v>
+      </c>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -3177,13 +3373,65 @@
       <c r="H11" s="2">
         <v>90</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="I11" s="2">
+        <v>90</v>
+      </c>
+      <c r="J11" s="2">
+        <v>93</v>
+      </c>
+      <c r="K11" s="2">
+        <v>93</v>
+      </c>
+      <c r="L11" s="2">
+        <v>93</v>
+      </c>
+      <c r="M11" s="2">
+        <v>96</v>
+      </c>
+      <c r="N11" s="2">
+        <v>100</v>
+      </c>
+      <c r="O11" s="2">
+        <v>100</v>
+      </c>
+      <c r="P11" s="9">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>96</v>
+      </c>
+      <c r="R11" s="7">
+        <v>96</v>
+      </c>
+      <c r="S11" s="7">
+        <v>90</v>
+      </c>
+      <c r="T11" s="7">
+        <v>87</v>
+      </c>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A11">

</xml_diff>

<commit_message>
selesai komputer hari ini
</commit_message>
<xml_diff>
--- a/pesantren/modul-komputer-mabaiz/penilaian.xlsx
+++ b/pesantren/modul-komputer-mabaiz/penilaian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZEN PROJECT\zen\pesantren\modul-komputer-mabaiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE52954A-7872-491F-B7F5-5C737A27A065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F841B2-1471-4999-9E04-1CA6046317E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="الاثنين" sheetId="5" r:id="rId1"/>
@@ -295,11 +295,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A19D3B-2FDF-4B23-B1AA-93203B194380}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="N13" sqref="N13"/>
     </sheetView>
@@ -594,69 +594,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1219,7 +1219,7 @@
       <c r="M13" s="8">
         <v>93</v>
       </c>
-      <c r="N13" s="17"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
@@ -1361,9 +1361,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8331428A-620A-44D2-9959-9DECEF50B2C0}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,69 +1372,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1510,7 +1510,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -1537,13 +1537,27 @@
       <c r="H4" s="2">
         <v>96</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
+      <c r="I4" s="2">
+        <v>86</v>
+      </c>
+      <c r="J4" s="2">
+        <v>86</v>
+      </c>
+      <c r="K4" s="2">
+        <v>86</v>
+      </c>
+      <c r="L4" s="2">
+        <v>80</v>
+      </c>
+      <c r="M4" s="2">
+        <v>90</v>
+      </c>
+      <c r="N4" s="7">
+        <v>96</v>
+      </c>
+      <c r="O4" s="2">
+        <v>93</v>
+      </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -1580,13 +1594,27 @@
       <c r="H5" s="2">
         <v>86</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="I5" s="2">
+        <v>86</v>
+      </c>
+      <c r="J5" s="3">
+        <v>90</v>
+      </c>
+      <c r="K5" s="3">
+        <v>86</v>
+      </c>
+      <c r="L5" s="3">
+        <v>90</v>
+      </c>
+      <c r="M5" s="2">
+        <v>83</v>
+      </c>
+      <c r="N5" s="2">
+        <v>90</v>
+      </c>
+      <c r="O5" s="3">
+        <v>90</v>
+      </c>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -1666,13 +1694,27 @@
       <c r="H7" s="2">
         <v>86</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
+      <c r="I7" s="2">
+        <v>80</v>
+      </c>
+      <c r="J7" s="2">
+        <v>93</v>
+      </c>
+      <c r="K7" s="5">
+        <v>90</v>
+      </c>
+      <c r="L7" s="5">
+        <v>80</v>
+      </c>
+      <c r="M7" s="2">
+        <v>93</v>
+      </c>
+      <c r="N7" s="2">
+        <v>83</v>
+      </c>
+      <c r="O7" s="2">
+        <v>80</v>
+      </c>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -1709,13 +1751,27 @@
       <c r="H8" s="3">
         <v>96</v>
       </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
+      <c r="I8" s="3">
+        <v>83</v>
+      </c>
+      <c r="J8" s="2">
+        <v>86</v>
+      </c>
+      <c r="K8" s="2">
+        <v>90</v>
+      </c>
+      <c r="L8" s="2">
+        <v>90</v>
+      </c>
+      <c r="M8" s="2">
+        <v>100</v>
+      </c>
+      <c r="N8" s="3">
+        <v>90</v>
+      </c>
+      <c r="O8" s="2">
+        <v>96</v>
+      </c>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
@@ -1751,13 +1807,27 @@
       <c r="H9" s="5">
         <v>80</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
+      <c r="I9" s="2">
+        <v>86</v>
+      </c>
+      <c r="J9" s="5">
+        <v>90</v>
+      </c>
+      <c r="K9" s="2">
+        <v>83</v>
+      </c>
+      <c r="L9" s="2">
+        <v>90</v>
+      </c>
+      <c r="M9" s="2">
+        <v>90</v>
+      </c>
+      <c r="N9" s="2">
+        <v>83</v>
+      </c>
+      <c r="O9" s="2">
+        <v>93</v>
+      </c>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
@@ -1793,13 +1863,27 @@
       <c r="H10" s="2">
         <v>93</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="I10" s="5">
+        <v>93</v>
+      </c>
+      <c r="J10" s="2">
+        <v>86</v>
+      </c>
+      <c r="K10" s="2">
+        <v>90</v>
+      </c>
+      <c r="L10" s="2">
+        <v>90</v>
+      </c>
+      <c r="M10" s="3">
+        <v>86</v>
+      </c>
+      <c r="N10" s="2">
+        <v>83</v>
+      </c>
+      <c r="O10" s="2">
+        <v>86</v>
+      </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
@@ -1835,13 +1919,27 @@
       <c r="H11" s="2">
         <v>100</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="I11" s="2">
+        <v>96</v>
+      </c>
+      <c r="J11" s="2">
+        <v>100</v>
+      </c>
+      <c r="K11" s="2">
+        <v>83</v>
+      </c>
+      <c r="L11" s="2">
+        <v>93</v>
+      </c>
+      <c r="M11" s="5">
+        <v>96</v>
+      </c>
+      <c r="N11" s="5">
+        <v>100</v>
+      </c>
+      <c r="O11" s="5">
+        <v>100</v>
+      </c>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
@@ -1877,13 +1975,27 @@
       <c r="H12" s="2">
         <v>93</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
+      <c r="I12" s="2">
+        <v>93</v>
+      </c>
+      <c r="J12" s="2">
+        <v>86</v>
+      </c>
+      <c r="K12" s="2">
+        <v>90</v>
+      </c>
+      <c r="L12" s="2">
+        <v>83</v>
+      </c>
+      <c r="M12" s="2">
+        <v>86</v>
+      </c>
+      <c r="N12" s="2">
+        <v>86</v>
+      </c>
+      <c r="O12" s="2">
+        <v>90</v>
+      </c>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
@@ -2160,69 +2272,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -2298,7 +2410,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -2891,69 +3003,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -3029,7 +3141,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -3575,69 +3687,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -3713,7 +3825,7 @@
       <c r="V3" s="2">
         <v>3</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="17"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">

</xml_diff>